<commit_message>
Updated ExcelApache and fixed some bugs
</commit_message>
<xml_diff>
--- a/Folha gerada.xlsx
+++ b/Folha gerada.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="72">
   <si>
     <t>Colaborador</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Referente ao mês:</t>
   </si>
   <si>
-    <t>setembro/2020</t>
+    <t>fevereiro/2020</t>
   </si>
   <si>
     <t>Dia do mês</t>
@@ -55,16 +55,43 @@
     <t>01</t>
   </si>
   <si>
+    <t>sábado</t>
+  </si>
+  <si>
+    <t>08:00 às 12:00</t>
+  </si>
+  <si>
+    <t>13:30 às 18:00</t>
+  </si>
+  <si>
+    <t>18:030 às 21:30</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>domingo</t>
+  </si>
+  <si>
+    <t>folga</t>
+  </si>
+  <si>
+    <t>---------------------</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>segunda</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
     <t>terça</t>
   </si>
   <si>
-    <t>folga</t>
-  </si>
-  <si>
-    <t>---------------------</t>
-  </si>
-  <si>
-    <t>02</t>
+    <t>05</t>
   </si>
   <si>
     <t>quarta</t>
@@ -73,7 +100,7 @@
     <t>08:00 às 13:00</t>
   </si>
   <si>
-    <t>03</t>
+    <t>06</t>
   </si>
   <si>
     <t>quinta</t>
@@ -85,39 +112,12 @@
     <t>18:00 às 21:30</t>
   </si>
   <si>
-    <t>04</t>
+    <t>07</t>
   </si>
   <si>
     <t>sexta</t>
   </si>
   <si>
-    <t>08:00 às 12:00</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>sábado</t>
-  </si>
-  <si>
-    <t>13:30 às 18:00</t>
-  </si>
-  <si>
-    <t>18:030 às 21:30</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>domingo</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>segunda</t>
-  </si>
-  <si>
     <t>08</t>
   </si>
   <si>
@@ -184,12 +184,6 @@
     <t>29</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
     <t>Faltas:</t>
   </si>
   <si>
@@ -214,28 +208,28 @@
     <t>CARLA</t>
   </si>
   <si>
+    <t>c08:00 às 12:00</t>
+  </si>
+  <si>
+    <t>13:30 às 18:30</t>
+  </si>
+  <si>
+    <t>cfolga</t>
+  </si>
+  <si>
     <t>c08:00 às 13:00</t>
   </si>
   <si>
-    <t>cfolga</t>
-  </si>
-  <si>
-    <t>c08:00 às 12:00</t>
-  </si>
-  <si>
-    <t>13:30 às 18:30</t>
-  </si>
-  <si>
     <t>MILENA</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>08:30 às 12:00</t>
+  </si>
+  <si>
     <t>18:00 às 21:00</t>
-  </si>
-  <si>
-    <t>08:30 às 12:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -601,7 +595,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -676,13 +670,13 @@
         <v>14</v>
       </c>
       <c r="D4" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s" s="2">
         <v>2</v>
@@ -690,22 +684,22 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s" s="3">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s" s="3">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s" s="2">
         <v>2</v>
@@ -713,22 +707,22 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="4">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s" s="2">
         <v>20</v>
-      </c>
-      <c r="C6" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s" s="3">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s" s="2">
-        <v>2</v>
       </c>
       <c r="G6" t="s" s="2">
         <v>2</v>
@@ -742,16 +736,16 @@
         <v>24</v>
       </c>
       <c r="C7" t="s" s="3">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s" s="3">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G7" t="s" s="2">
         <v>2</v>
@@ -759,19 +753,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="4">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s" s="3">
         <v>26</v>
       </c>
-      <c r="B8" t="s" s="3">
+      <c r="C8" t="s" s="3">
         <v>27</v>
       </c>
-      <c r="C8" t="s" s="3">
-        <v>25</v>
-      </c>
       <c r="D8" t="s" s="3">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s" s="3">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s" s="2">
         <v>2</v>
@@ -782,22 +776,22 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="4">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s" s="3">
         <v>30</v>
       </c>
-      <c r="B9" t="s" s="3">
+      <c r="E9" t="s" s="3">
         <v>31</v>
       </c>
-      <c r="C9" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s" s="3">
-        <v>14</v>
-      </c>
       <c r="F9" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G9" t="s" s="2">
         <v>2</v>
@@ -814,13 +808,13 @@
         <v>14</v>
       </c>
       <c r="D10" t="s" s="3">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s" s="3">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G10" t="s" s="2">
         <v>2</v>
@@ -837,13 +831,13 @@
         <v>14</v>
       </c>
       <c r="D11" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G11" t="s" s="2">
         <v>2</v>
@@ -854,19 +848,19 @@
         <v>35</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s" s="3">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s" s="3">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G12" t="s" s="2">
         <v>2</v>
@@ -877,19 +871,19 @@
         <v>36</v>
       </c>
       <c r="B13" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s" s="2">
         <v>20</v>
-      </c>
-      <c r="C13" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s" s="3">
-        <v>22</v>
-      </c>
-      <c r="F13" t="s" s="2">
-        <v>2</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>2</v>
@@ -903,16 +897,16 @@
         <v>24</v>
       </c>
       <c r="C14" t="s" s="3">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s" s="3">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G14" t="s" s="2">
         <v>2</v>
@@ -923,16 +917,16 @@
         <v>38</v>
       </c>
       <c r="B15" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s" s="3">
         <v>27</v>
       </c>
-      <c r="C15" t="s" s="3">
-        <v>25</v>
-      </c>
       <c r="D15" t="s" s="3">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s" s="3">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F15" t="s" s="2">
         <v>2</v>
@@ -946,19 +940,19 @@
         <v>39</v>
       </c>
       <c r="B16" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s" s="3">
         <v>31</v>
       </c>
-      <c r="C16" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D16" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="E16" t="s" s="3">
-        <v>14</v>
-      </c>
       <c r="F16" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G16" t="s" s="2">
         <v>2</v>
@@ -975,13 +969,13 @@
         <v>14</v>
       </c>
       <c r="D17" t="s" s="3">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s" s="3">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>2</v>
@@ -998,13 +992,13 @@
         <v>14</v>
       </c>
       <c r="D18" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>2</v>
@@ -1015,19 +1009,19 @@
         <v>42</v>
       </c>
       <c r="B19" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s" s="3">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E19" t="s" s="3">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G19" t="s" s="2">
         <v>2</v>
@@ -1038,19 +1032,19 @@
         <v>43</v>
       </c>
       <c r="B20" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s" s="2">
         <v>20</v>
-      </c>
-      <c r="C20" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D20" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="E20" t="s" s="3">
-        <v>22</v>
-      </c>
-      <c r="F20" t="s" s="2">
-        <v>2</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>2</v>
@@ -1064,16 +1058,16 @@
         <v>24</v>
       </c>
       <c r="C21" t="s" s="3">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D21" t="s" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s" s="3">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G21" t="s" s="2">
         <v>2</v>
@@ -1084,16 +1078,16 @@
         <v>45</v>
       </c>
       <c r="B22" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s" s="3">
         <v>27</v>
       </c>
-      <c r="C22" t="s" s="3">
-        <v>25</v>
-      </c>
       <c r="D22" t="s" s="3">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E22" t="s" s="3">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F22" t="s" s="2">
         <v>2</v>
@@ -1107,19 +1101,19 @@
         <v>46</v>
       </c>
       <c r="B23" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s" s="3">
         <v>31</v>
       </c>
-      <c r="C23" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D23" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="E23" t="s" s="3">
-        <v>14</v>
-      </c>
       <c r="F23" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>2</v>
@@ -1136,13 +1130,13 @@
         <v>14</v>
       </c>
       <c r="D24" t="s" s="3">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E24" t="s" s="3">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G24" t="s" s="2">
         <v>2</v>
@@ -1159,13 +1153,13 @@
         <v>14</v>
       </c>
       <c r="D25" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G25" t="s" s="2">
         <v>2</v>
@@ -1176,19 +1170,19 @@
         <v>49</v>
       </c>
       <c r="B26" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s" s="3">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E26" t="s" s="3">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>2</v>
@@ -1199,19 +1193,19 @@
         <v>50</v>
       </c>
       <c r="B27" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="D27" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="E27" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="F27" t="s" s="2">
         <v>20</v>
-      </c>
-      <c r="C27" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D27" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="E27" t="s" s="3">
-        <v>22</v>
-      </c>
-      <c r="F27" t="s" s="2">
-        <v>2</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>2</v>
@@ -1225,16 +1219,16 @@
         <v>24</v>
       </c>
       <c r="C28" t="s" s="3">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D28" t="s" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E28" t="s" s="3">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>2</v>
@@ -1245,16 +1239,16 @@
         <v>52</v>
       </c>
       <c r="B29" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s" s="3">
         <v>27</v>
       </c>
-      <c r="C29" t="s" s="3">
-        <v>25</v>
-      </c>
       <c r="D29" t="s" s="3">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E29" t="s" s="3">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F29" t="s" s="2">
         <v>2</v>
@@ -1268,19 +1262,19 @@
         <v>53</v>
       </c>
       <c r="B30" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="D30" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="E30" t="s" s="3">
         <v>31</v>
       </c>
-      <c r="C30" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D30" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="E30" t="s" s="3">
-        <v>14</v>
-      </c>
       <c r="F30" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>2</v>
@@ -1297,13 +1291,13 @@
         <v>14</v>
       </c>
       <c r="D31" t="s" s="3">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E31" t="s" s="3">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>2</v>
@@ -1320,121 +1314,46 @@
         <v>14</v>
       </c>
       <c r="D32" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E32" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="s" s="4">
-        <v>56</v>
-      </c>
-      <c r="B33" t="s" s="3">
-        <v>17</v>
-      </c>
-      <c r="C33" t="s" s="3">
-        <v>18</v>
-      </c>
-      <c r="D33" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="E33" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="F33" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="G33" t="s" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s" s="4">
-        <v>57</v>
-      </c>
-      <c r="B34" t="s" s="3">
-        <v>33</v>
-      </c>
-      <c r="C34" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D34" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="E34" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="F34" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="G34" t="s" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s" s="6">
-        <v>58</v>
-      </c>
-      <c r="B38" t="s" s="5">
-        <v>59</v>
-      </c>
-      <c r="C38" t="s" s="5">
-        <v>60</v>
-      </c>
-      <c r="D38" t="s" s="5">
-        <v>2</v>
-      </c>
-      <c r="E38" t="s" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s" s="11">
-        <v>2</v>
-      </c>
-      <c r="E39" t="s" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s" s="11">
-        <v>61</v>
-      </c>
-      <c r="C40" t="s" s="13">
-        <v>62</v>
-      </c>
-      <c r="E40" t="s" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s" s="11">
-        <v>2</v>
-      </c>
-      <c r="E41" t="s" s="12">
-        <v>2</v>
-      </c>
-    </row>
     <row r="42">
-      <c r="A42" t="s" s="11">
-        <v>63</v>
-      </c>
-      <c r="C42" t="s" s="13">
-        <v>62</v>
-      </c>
-      <c r="E42" t="s" s="12">
+      <c r="A42" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s" s="5">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s" s="5">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s" s="5">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="11">
+        <v>56</v>
+      </c>
+      <c r="B43" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="C43" t="s" s="13">
+        <v>58</v>
+      </c>
+      <c r="D43" t="s" s="13">
         <v>2</v>
       </c>
       <c r="E43" t="s" s="12">
@@ -1442,19 +1361,65 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s" s="9">
-        <v>64</v>
-      </c>
-      <c r="B44" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="C44" t="s" s="8">
+      <c r="A44" t="s" s="11">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="11">
+        <v>59</v>
+      </c>
+      <c r="C45" t="s" s="13">
+        <v>60</v>
+      </c>
+      <c r="E45" t="s" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="11">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="11">
+        <v>61</v>
+      </c>
+      <c r="C47" t="s" s="13">
+        <v>60</v>
+      </c>
+      <c r="E47" t="s" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="11">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="9">
         <v>62</v>
       </c>
-      <c r="D44" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E44" t="s" s="10">
+      <c r="B49" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s" s="8">
+        <v>60</v>
+      </c>
+      <c r="D49" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s" s="10">
         <v>2</v>
       </c>
     </row>
@@ -1469,7 +1434,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1493,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s" s="12">
         <v>2</v>
@@ -1541,16 +1506,16 @@
         <v>13</v>
       </c>
       <c r="C4" t="s" s="3">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s" s="2">
         <v>2</v>
@@ -1558,19 +1523,19 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s" s="3">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s" s="3">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s" s="3">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s" s="2">
         <v>2</v>
@@ -1581,22 +1546,22 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="4">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s" s="3">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s" s="2">
         <v>20</v>
-      </c>
-      <c r="C6" t="s" s="3">
-        <v>67</v>
-      </c>
-      <c r="D6" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s" s="3">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s" s="2">
-        <v>2</v>
       </c>
       <c r="G6" t="s" s="2">
         <v>2</v>
@@ -1610,16 +1575,16 @@
         <v>24</v>
       </c>
       <c r="C7" t="s" s="3">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s" s="3">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G7" t="s" s="2">
         <v>2</v>
@@ -1627,19 +1592,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="4">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s" s="3">
         <v>26</v>
       </c>
-      <c r="B8" t="s" s="3">
-        <v>27</v>
-      </c>
       <c r="C8" t="s" s="3">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s" s="3">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s" s="3">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s" s="2">
         <v>2</v>
@@ -1650,19 +1615,19 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="4">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s" s="3">
+        <v>66</v>
+      </c>
+      <c r="D9" t="s" s="3">
         <v>30</v>
       </c>
-      <c r="B9" t="s" s="3">
+      <c r="E9" t="s" s="3">
         <v>31</v>
-      </c>
-      <c r="C9" t="s" s="3">
-        <v>68</v>
-      </c>
-      <c r="D9" t="s" s="3">
-        <v>69</v>
-      </c>
-      <c r="E9" t="s" s="3">
-        <v>14</v>
       </c>
       <c r="F9" t="s" s="2">
         <v>2</v>
@@ -1679,16 +1644,16 @@
         <v>33</v>
       </c>
       <c r="C10" t="s" s="3">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s" s="3">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s" s="3">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G10" t="s" s="2">
         <v>2</v>
@@ -1702,16 +1667,16 @@
         <v>13</v>
       </c>
       <c r="C11" t="s" s="3">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G11" t="s" s="2">
         <v>2</v>
@@ -1722,16 +1687,16 @@
         <v>35</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s" s="3">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s" s="3">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s" s="3">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s" s="2">
         <v>2</v>
@@ -1745,19 +1710,19 @@
         <v>36</v>
       </c>
       <c r="B13" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s" s="3">
+        <v>66</v>
+      </c>
+      <c r="D13" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s" s="2">
         <v>20</v>
-      </c>
-      <c r="C13" t="s" s="3">
-        <v>67</v>
-      </c>
-      <c r="D13" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s" s="3">
-        <v>22</v>
-      </c>
-      <c r="F13" t="s" s="2">
-        <v>2</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>2</v>
@@ -1771,16 +1736,16 @@
         <v>24</v>
       </c>
       <c r="C14" t="s" s="3">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s" s="3">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G14" t="s" s="2">
         <v>2</v>
@@ -1791,16 +1756,16 @@
         <v>38</v>
       </c>
       <c r="B15" t="s" s="3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s" s="3">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s" s="3">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s" s="3">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F15" t="s" s="2">
         <v>2</v>
@@ -1814,16 +1779,16 @@
         <v>39</v>
       </c>
       <c r="B16" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s" s="3">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s" s="3">
         <v>31</v>
-      </c>
-      <c r="C16" t="s" s="3">
-        <v>68</v>
-      </c>
-      <c r="D16" t="s" s="3">
-        <v>69</v>
-      </c>
-      <c r="E16" t="s" s="3">
-        <v>14</v>
       </c>
       <c r="F16" t="s" s="2">
         <v>2</v>
@@ -1840,16 +1805,16 @@
         <v>33</v>
       </c>
       <c r="C17" t="s" s="3">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D17" t="s" s="3">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s" s="3">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>2</v>
@@ -1863,16 +1828,16 @@
         <v>13</v>
       </c>
       <c r="C18" t="s" s="3">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>2</v>
@@ -1883,16 +1848,16 @@
         <v>42</v>
       </c>
       <c r="B19" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s" s="3">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s" s="3">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s" s="3">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F19" t="s" s="2">
         <v>2</v>
@@ -1906,19 +1871,19 @@
         <v>43</v>
       </c>
       <c r="B20" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s" s="3">
+        <v>66</v>
+      </c>
+      <c r="D20" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s" s="2">
         <v>20</v>
-      </c>
-      <c r="C20" t="s" s="3">
-        <v>67</v>
-      </c>
-      <c r="D20" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="E20" t="s" s="3">
-        <v>22</v>
-      </c>
-      <c r="F20" t="s" s="2">
-        <v>2</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>2</v>
@@ -1932,16 +1897,16 @@
         <v>24</v>
       </c>
       <c r="C21" t="s" s="3">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="D21" t="s" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s" s="3">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G21" t="s" s="2">
         <v>2</v>
@@ -1952,16 +1917,16 @@
         <v>45</v>
       </c>
       <c r="B22" t="s" s="3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s" s="3">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s" s="3">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E22" t="s" s="3">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F22" t="s" s="2">
         <v>2</v>
@@ -1975,16 +1940,16 @@
         <v>46</v>
       </c>
       <c r="B23" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s" s="3">
+        <v>66</v>
+      </c>
+      <c r="D23" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s" s="3">
         <v>31</v>
-      </c>
-      <c r="C23" t="s" s="3">
-        <v>68</v>
-      </c>
-      <c r="D23" t="s" s="3">
-        <v>69</v>
-      </c>
-      <c r="E23" t="s" s="3">
-        <v>14</v>
       </c>
       <c r="F23" t="s" s="2">
         <v>2</v>
@@ -2001,16 +1966,16 @@
         <v>33</v>
       </c>
       <c r="C24" t="s" s="3">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D24" t="s" s="3">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E24" t="s" s="3">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G24" t="s" s="2">
         <v>2</v>
@@ -2024,16 +1989,16 @@
         <v>13</v>
       </c>
       <c r="C25" t="s" s="3">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="D25" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G25" t="s" s="2">
         <v>2</v>
@@ -2044,16 +2009,16 @@
         <v>49</v>
       </c>
       <c r="B26" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s" s="3">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D26" t="s" s="3">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="E26" t="s" s="3">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F26" t="s" s="2">
         <v>2</v>
@@ -2067,19 +2032,19 @@
         <v>50</v>
       </c>
       <c r="B27" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s" s="3">
+        <v>66</v>
+      </c>
+      <c r="D27" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="E27" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="F27" t="s" s="2">
         <v>20</v>
-      </c>
-      <c r="C27" t="s" s="3">
-        <v>67</v>
-      </c>
-      <c r="D27" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="E27" t="s" s="3">
-        <v>22</v>
-      </c>
-      <c r="F27" t="s" s="2">
-        <v>2</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>2</v>
@@ -2093,16 +2058,16 @@
         <v>24</v>
       </c>
       <c r="C28" t="s" s="3">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="D28" t="s" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E28" t="s" s="3">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>2</v>
@@ -2113,16 +2078,16 @@
         <v>52</v>
       </c>
       <c r="B29" t="s" s="3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s" s="3">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D29" t="s" s="3">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E29" t="s" s="3">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F29" t="s" s="2">
         <v>2</v>
@@ -2136,16 +2101,16 @@
         <v>53</v>
       </c>
       <c r="B30" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s" s="3">
+        <v>66</v>
+      </c>
+      <c r="D30" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="E30" t="s" s="3">
         <v>31</v>
-      </c>
-      <c r="C30" t="s" s="3">
-        <v>68</v>
-      </c>
-      <c r="D30" t="s" s="3">
-        <v>69</v>
-      </c>
-      <c r="E30" t="s" s="3">
-        <v>14</v>
       </c>
       <c r="F30" t="s" s="2">
         <v>2</v>
@@ -2162,16 +2127,16 @@
         <v>33</v>
       </c>
       <c r="C31" t="s" s="3">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D31" t="s" s="3">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E31" t="s" s="3">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>2</v>
@@ -2185,124 +2150,49 @@
         <v>13</v>
       </c>
       <c r="C32" t="s" s="3">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="D32" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E32" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="s" s="4">
-        <v>56</v>
-      </c>
-      <c r="B33" t="s" s="3">
-        <v>17</v>
-      </c>
-      <c r="C33" t="s" s="3">
-        <v>66</v>
-      </c>
-      <c r="D33" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="E33" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="F33" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="G33" t="s" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s" s="4">
-        <v>57</v>
-      </c>
-      <c r="B34" t="s" s="3">
-        <v>33</v>
-      </c>
-      <c r="C34" t="s" s="3">
-        <v>67</v>
-      </c>
-      <c r="D34" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="E34" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="F34" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="G34" t="s" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s" s="6">
-        <v>58</v>
-      </c>
-      <c r="B38" t="s" s="5">
-        <v>59</v>
-      </c>
-      <c r="C38" t="s" s="5">
-        <v>60</v>
-      </c>
-      <c r="D38" t="s" s="5">
-        <v>2</v>
-      </c>
-      <c r="E38" t="s" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s" s="11">
-        <v>2</v>
-      </c>
-      <c r="E39" t="s" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s" s="11">
-        <v>61</v>
-      </c>
-      <c r="C40" t="s" s="13">
-        <v>62</v>
-      </c>
-      <c r="E40" t="s" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s" s="11">
-        <v>2</v>
-      </c>
-      <c r="E41" t="s" s="12">
-        <v>2</v>
-      </c>
-    </row>
     <row r="42">
-      <c r="A42" t="s" s="11">
-        <v>63</v>
-      </c>
-      <c r="C42" t="s" s="13">
-        <v>62</v>
-      </c>
-      <c r="E42" t="s" s="12">
+      <c r="A42" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s" s="5">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s" s="5">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s" s="5">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="11">
+        <v>56</v>
+      </c>
+      <c r="B43" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="C43" t="s" s="13">
+        <v>58</v>
+      </c>
+      <c r="D43" t="s" s="13">
         <v>2</v>
       </c>
       <c r="E43" t="s" s="12">
@@ -2310,19 +2200,65 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s" s="9">
-        <v>64</v>
-      </c>
-      <c r="B44" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="C44" t="s" s="8">
+      <c r="A44" t="s" s="11">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="11">
+        <v>59</v>
+      </c>
+      <c r="C45" t="s" s="13">
+        <v>60</v>
+      </c>
+      <c r="E45" t="s" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="11">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="11">
+        <v>61</v>
+      </c>
+      <c r="C47" t="s" s="13">
+        <v>60</v>
+      </c>
+      <c r="E47" t="s" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="11">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="9">
         <v>62</v>
       </c>
-      <c r="D44" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E44" t="s" s="10">
+      <c r="B49" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s" s="8">
+        <v>60</v>
+      </c>
+      <c r="D49" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s" s="10">
         <v>2</v>
       </c>
     </row>
@@ -2337,7 +2273,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2361,7 +2297,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G1" t="s" s="12">
         <v>2</v>
@@ -2412,13 +2348,13 @@
         <v>14</v>
       </c>
       <c r="D4" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s" s="2">
         <v>2</v>
@@ -2426,19 +2362,19 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s" s="3">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s" s="3">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s" s="2">
         <v>2</v>
@@ -2449,22 +2385,22 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="4">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s" s="2">
         <v>20</v>
-      </c>
-      <c r="C6" t="s" s="3">
-        <v>72</v>
-      </c>
-      <c r="D6" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s" s="3">
-        <v>73</v>
-      </c>
-      <c r="F6" t="s" s="2">
-        <v>2</v>
       </c>
       <c r="G6" t="s" s="2">
         <v>2</v>
@@ -2478,16 +2414,16 @@
         <v>24</v>
       </c>
       <c r="C7" t="s" s="3">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s" s="3">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s" s="3">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G7" t="s" s="2">
         <v>2</v>
@@ -2495,19 +2431,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="4">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s" s="3">
         <v>26</v>
       </c>
-      <c r="B8" t="s" s="3">
-        <v>27</v>
-      </c>
       <c r="C8" t="s" s="3">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s" s="3">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s" s="3">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F8" t="s" s="2">
         <v>2</v>
@@ -2518,19 +2454,19 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="4">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s" s="3">
+        <v>70</v>
+      </c>
+      <c r="D9" t="s" s="3">
         <v>30</v>
       </c>
-      <c r="B9" t="s" s="3">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s" s="3">
-        <v>72</v>
-      </c>
-      <c r="D9" t="s" s="3">
-        <v>14</v>
-      </c>
       <c r="E9" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F9" t="s" s="2">
         <v>2</v>
@@ -2547,16 +2483,16 @@
         <v>33</v>
       </c>
       <c r="C10" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G10" t="s" s="2">
         <v>2</v>
@@ -2573,13 +2509,13 @@
         <v>14</v>
       </c>
       <c r="D11" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G11" t="s" s="2">
         <v>2</v>
@@ -2590,16 +2526,16 @@
         <v>35</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s" s="3">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s" s="3">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s" s="2">
         <v>2</v>
@@ -2613,19 +2549,19 @@
         <v>36</v>
       </c>
       <c r="B13" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s" s="2">
         <v>20</v>
-      </c>
-      <c r="C13" t="s" s="3">
-        <v>72</v>
-      </c>
-      <c r="D13" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s" s="3">
-        <v>73</v>
-      </c>
-      <c r="F13" t="s" s="2">
-        <v>2</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>2</v>
@@ -2639,16 +2575,16 @@
         <v>24</v>
       </c>
       <c r="C14" t="s" s="3">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s" s="3">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s" s="3">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G14" t="s" s="2">
         <v>2</v>
@@ -2659,16 +2595,16 @@
         <v>38</v>
       </c>
       <c r="B15" t="s" s="3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s" s="3">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s" s="3">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="E15" t="s" s="3">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F15" t="s" s="2">
         <v>2</v>
@@ -2682,16 +2618,16 @@
         <v>39</v>
       </c>
       <c r="B16" t="s" s="3">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s" s="3">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s" s="3">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F16" t="s" s="2">
         <v>2</v>
@@ -2708,16 +2644,16 @@
         <v>33</v>
       </c>
       <c r="C17" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>2</v>
@@ -2734,13 +2670,13 @@
         <v>14</v>
       </c>
       <c r="D18" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>2</v>
@@ -2751,16 +2687,16 @@
         <v>42</v>
       </c>
       <c r="B19" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s" s="3">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="D19" t="s" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E19" t="s" s="3">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="F19" t="s" s="2">
         <v>2</v>
@@ -2774,19 +2710,19 @@
         <v>43</v>
       </c>
       <c r="B20" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s" s="2">
         <v>20</v>
-      </c>
-      <c r="C20" t="s" s="3">
-        <v>72</v>
-      </c>
-      <c r="D20" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="E20" t="s" s="3">
-        <v>73</v>
-      </c>
-      <c r="F20" t="s" s="2">
-        <v>2</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>2</v>
@@ -2800,16 +2736,16 @@
         <v>24</v>
       </c>
       <c r="C21" t="s" s="3">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="D21" t="s" s="3">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s" s="3">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G21" t="s" s="2">
         <v>2</v>
@@ -2820,16 +2756,16 @@
         <v>45</v>
       </c>
       <c r="B22" t="s" s="3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s" s="3">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D22" t="s" s="3">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s" s="3">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F22" t="s" s="2">
         <v>2</v>
@@ -2843,16 +2779,16 @@
         <v>46</v>
       </c>
       <c r="B23" t="s" s="3">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s" s="3">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s" s="3">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E23" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F23" t="s" s="2">
         <v>2</v>
@@ -2869,16 +2805,16 @@
         <v>33</v>
       </c>
       <c r="C24" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G24" t="s" s="2">
         <v>2</v>
@@ -2895,13 +2831,13 @@
         <v>14</v>
       </c>
       <c r="D25" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="E25" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G25" t="s" s="2">
         <v>2</v>
@@ -2912,16 +2848,16 @@
         <v>49</v>
       </c>
       <c r="B26" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s" s="3">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="D26" t="s" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E26" t="s" s="3">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="F26" t="s" s="2">
         <v>2</v>
@@ -2935,19 +2871,19 @@
         <v>50</v>
       </c>
       <c r="B27" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="D27" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="E27" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="F27" t="s" s="2">
         <v>20</v>
-      </c>
-      <c r="C27" t="s" s="3">
-        <v>72</v>
-      </c>
-      <c r="D27" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="E27" t="s" s="3">
-        <v>73</v>
-      </c>
-      <c r="F27" t="s" s="2">
-        <v>2</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>2</v>
@@ -2961,16 +2897,16 @@
         <v>24</v>
       </c>
       <c r="C28" t="s" s="3">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="D28" t="s" s="3">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="E28" t="s" s="3">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>2</v>
@@ -2981,16 +2917,16 @@
         <v>52</v>
       </c>
       <c r="B29" t="s" s="3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s" s="3">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D29" t="s" s="3">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="E29" t="s" s="3">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F29" t="s" s="2">
         <v>2</v>
@@ -3004,16 +2940,16 @@
         <v>53</v>
       </c>
       <c r="B30" t="s" s="3">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s" s="3">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D30" t="s" s="3">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E30" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F30" t="s" s="2">
         <v>2</v>
@@ -3030,16 +2966,16 @@
         <v>33</v>
       </c>
       <c r="C31" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="D31" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="E31" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>2</v>
@@ -3056,121 +2992,46 @@
         <v>14</v>
       </c>
       <c r="D32" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="E32" t="s" s="3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="s" s="4">
-        <v>56</v>
-      </c>
-      <c r="B33" t="s" s="3">
-        <v>17</v>
-      </c>
-      <c r="C33" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D33" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="E33" t="s" s="3">
-        <v>71</v>
-      </c>
-      <c r="F33" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="G33" t="s" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s" s="4">
-        <v>57</v>
-      </c>
-      <c r="B34" t="s" s="3">
-        <v>33</v>
-      </c>
-      <c r="C34" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D34" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="E34" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="F34" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="G34" t="s" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s" s="6">
-        <v>58</v>
-      </c>
-      <c r="B38" t="s" s="5">
-        <v>59</v>
-      </c>
-      <c r="C38" t="s" s="5">
-        <v>60</v>
-      </c>
-      <c r="D38" t="s" s="5">
-        <v>2</v>
-      </c>
-      <c r="E38" t="s" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s" s="11">
-        <v>2</v>
-      </c>
-      <c r="E39" t="s" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s" s="11">
-        <v>61</v>
-      </c>
-      <c r="C40" t="s" s="13">
-        <v>62</v>
-      </c>
-      <c r="E40" t="s" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s" s="11">
-        <v>2</v>
-      </c>
-      <c r="E41" t="s" s="12">
-        <v>2</v>
-      </c>
-    </row>
     <row r="42">
-      <c r="A42" t="s" s="11">
-        <v>63</v>
-      </c>
-      <c r="C42" t="s" s="13">
-        <v>62</v>
-      </c>
-      <c r="E42" t="s" s="12">
+      <c r="A42" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s" s="5">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s" s="5">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s" s="5">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="11">
+        <v>56</v>
+      </c>
+      <c r="B43" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="C43" t="s" s="13">
+        <v>58</v>
+      </c>
+      <c r="D43" t="s" s="13">
         <v>2</v>
       </c>
       <c r="E43" t="s" s="12">
@@ -3178,19 +3039,65 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s" s="9">
-        <v>64</v>
-      </c>
-      <c r="B44" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="C44" t="s" s="8">
+      <c r="A44" t="s" s="11">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="11">
+        <v>59</v>
+      </c>
+      <c r="C45" t="s" s="13">
+        <v>60</v>
+      </c>
+      <c r="E45" t="s" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="11">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="11">
+        <v>61</v>
+      </c>
+      <c r="C47" t="s" s="13">
+        <v>60</v>
+      </c>
+      <c r="E47" t="s" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="11">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="9">
         <v>62</v>
       </c>
-      <c r="D44" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E44" t="s" s="10">
+      <c r="B49" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s" s="8">
+        <v>60</v>
+      </c>
+      <c r="D49" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s" s="10">
         <v>2</v>
       </c>
     </row>

</xml_diff>